<commit_message>
correcting rounding checks and updating data
</commit_message>
<xml_diff>
--- a/rawdata/VZ_StateMinimumWage_Changes.xlsx
+++ b/rawdata/VZ_StateMinimumWage_Changes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1289" uniqueCount="498">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1290" uniqueCount="499">
   <si>
     <t xml:space="preserve">statefips</t>
   </si>
@@ -1451,6 +1451,9 @@
   </si>
   <si>
     <t xml:space="preserve">West Virginia - State Website - Minimum Wage History - 01.14.2028</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abovestate</t>
   </si>
   <si>
     <t xml:space="preserve">West Virginia - State Website - Minimum Wage History - 01.14.2029</t>
@@ -1609,7 +1612,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1642,10 +1645,6 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -1665,18 +1664,18 @@
   </sheetPr>
   <dimension ref="1:595"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A321" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E340" activeCellId="0" sqref="E340"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A477" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F389" activeCellId="0" sqref="F389"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="2" style="2" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="2" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="1022" min="12" style="2" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="2" style="2" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="2" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="1022" min="12" style="2" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9987,7 +9986,7 @@
       <c r="K303" s="0"/>
     </row>
     <row r="304" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A304" s="8" t="n">
+      <c r="A304" s="6" t="n">
         <v>29</v>
       </c>
       <c r="B304" s="2" t="s">
@@ -10010,6 +10009,7 @@
       <c r="I304" s="2" t="s">
         <v>243</v>
       </c>
+      <c r="J304" s="0"/>
       <c r="K304" s="0"/>
     </row>
     <row r="305" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10664,7 +10664,7 @@
       <c r="K327" s="0"/>
     </row>
     <row r="328" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A328" s="8" t="n">
+      <c r="A328" s="6" t="n">
         <v>30</v>
       </c>
       <c r="B328" s="2" t="s">
@@ -10689,6 +10689,7 @@
       <c r="I328" s="2" t="s">
         <v>267</v>
       </c>
+      <c r="J328" s="0"/>
       <c r="K328" s="0"/>
     </row>
     <row r="329" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13876,6 +13877,7 @@
       <c r="I448" s="2" t="s">
         <v>372</v>
       </c>
+      <c r="J448" s="0"/>
       <c r="K448" s="0"/>
     </row>
     <row r="449" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13901,6 +13903,7 @@
       <c r="I449" s="2" t="s">
         <v>372</v>
       </c>
+      <c r="J449" s="0"/>
       <c r="K449" s="0"/>
     </row>
     <row r="450" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13926,6 +13929,7 @@
       <c r="I450" s="2" t="s">
         <v>372</v>
       </c>
+      <c r="J450" s="0"/>
       <c r="K450" s="0"/>
     </row>
     <row r="451" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13951,6 +13955,7 @@
       <c r="I451" s="2" t="s">
         <v>372</v>
       </c>
+      <c r="J451" s="0"/>
       <c r="K451" s="0"/>
     </row>
     <row r="452" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13976,6 +13981,7 @@
       <c r="I452" s="2" t="s">
         <v>372</v>
       </c>
+      <c r="J452" s="0"/>
       <c r="K452" s="0"/>
     </row>
     <row r="453" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14001,6 +14007,7 @@
       <c r="I453" s="2" t="s">
         <v>372</v>
       </c>
+      <c r="J453" s="0"/>
       <c r="K453" s="0"/>
     </row>
     <row r="454" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14026,6 +14033,7 @@
       <c r="I454" s="2" t="s">
         <v>372</v>
       </c>
+      <c r="J454" s="0"/>
       <c r="K454" s="0"/>
     </row>
     <row r="455" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14975,7 +14983,7 @@
       <c r="K491" s="0"/>
     </row>
     <row r="492" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A492" s="8" t="n">
+      <c r="A492" s="6" t="n">
         <v>44</v>
       </c>
       <c r="B492" s="2" t="s">
@@ -15104,7 +15112,7 @@
       <c r="K496" s="0"/>
     </row>
     <row r="497" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A497" s="8" t="n">
+      <c r="A497" s="6" t="n">
         <v>46</v>
       </c>
       <c r="B497" s="2" t="s">
@@ -15125,6 +15133,7 @@
       <c r="I497" s="2" t="s">
         <v>415</v>
       </c>
+      <c r="J497" s="0"/>
       <c r="K497" s="0"/>
     </row>
     <row r="498" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16997,14 +17006,14 @@
       <c r="D573" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="E573" s="2" t="n">
-        <v>1</v>
+      <c r="E573" s="2" t="s">
+        <v>477</v>
       </c>
       <c r="F573" s="2" t="n">
         <v>5.85</v>
       </c>
       <c r="I573" s="2" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="J573" s="0"/>
     </row>
@@ -17028,7 +17037,7 @@
         <v>6.55</v>
       </c>
       <c r="I574" s="2" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="J574" s="0"/>
     </row>
@@ -17052,12 +17061,12 @@
         <v>7.25</v>
       </c>
       <c r="I575" s="2" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="J575" s="0"/>
     </row>
     <row r="576" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A576" s="8" t="n">
+      <c r="A576" s="6" t="n">
         <v>54</v>
       </c>
       <c r="B576" s="2" t="s">
@@ -17076,12 +17085,12 @@
         <v>8</v>
       </c>
       <c r="I576" s="2" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="J576" s="0"/>
     </row>
     <row r="577" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A577" s="8" t="n">
+      <c r="A577" s="6" t="n">
         <v>54</v>
       </c>
       <c r="B577" s="2" t="s">
@@ -17100,7 +17109,7 @@
         <v>8.75</v>
       </c>
       <c r="I577" s="2" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="J577" s="0"/>
     </row>
@@ -17135,7 +17144,7 @@
         <v>55</v>
       </c>
       <c r="B579" s="2" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="C579" s="2" t="n">
         <v>1975</v>
@@ -17150,7 +17159,7 @@
         <v>2</v>
       </c>
       <c r="I579" s="2" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="J579" s="0"/>
     </row>
@@ -17159,7 +17168,7 @@
         <v>55</v>
       </c>
       <c r="B580" s="2" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="C580" s="2" t="n">
         <v>1976</v>
@@ -17174,7 +17183,7 @@
         <v>2.1</v>
       </c>
       <c r="I580" s="2" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="J580" s="0"/>
     </row>
@@ -17183,7 +17192,7 @@
         <v>55</v>
       </c>
       <c r="B581" s="2" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="C581" s="2" t="n">
         <v>1977</v>
@@ -17198,7 +17207,7 @@
         <v>2.2</v>
       </c>
       <c r="I581" s="2" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="J581" s="0"/>
     </row>
@@ -17207,7 +17216,7 @@
         <v>55</v>
       </c>
       <c r="B582" s="2" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="C582" s="2" t="n">
         <v>1978</v>
@@ -17222,7 +17231,7 @@
         <v>2.55</v>
       </c>
       <c r="I582" s="2" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="J582" s="0"/>
     </row>
@@ -17231,7 +17240,7 @@
         <v>55</v>
       </c>
       <c r="B583" s="2" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="C583" s="2" t="n">
         <v>1979</v>
@@ -17246,7 +17255,7 @@
         <v>2.8</v>
       </c>
       <c r="I583" s="2" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="J583" s="0"/>
     </row>
@@ -17255,7 +17264,7 @@
         <v>55</v>
       </c>
       <c r="B584" s="2" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="C584" s="2" t="n">
         <v>1980</v>
@@ -17270,7 +17279,7 @@
         <v>3</v>
       </c>
       <c r="I584" s="2" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="J584" s="0"/>
     </row>
@@ -17279,7 +17288,7 @@
         <v>55</v>
       </c>
       <c r="B585" s="2" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="C585" s="2" t="n">
         <v>1981</v>
@@ -17294,7 +17303,7 @@
         <v>3.25</v>
       </c>
       <c r="I585" s="2" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="J585" s="0"/>
     </row>
@@ -17303,7 +17312,7 @@
         <v>55</v>
       </c>
       <c r="B586" s="2" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="C586" s="2" t="n">
         <v>1987</v>
@@ -17318,7 +17327,7 @@
         <v>3.35</v>
       </c>
       <c r="I586" s="2" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="J586" s="0"/>
     </row>
@@ -17327,7 +17336,7 @@
         <v>55</v>
       </c>
       <c r="B587" s="2" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="C587" s="2" t="n">
         <v>1989</v>
@@ -17342,7 +17351,7 @@
         <v>3.65</v>
       </c>
       <c r="I587" s="2" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="J587" s="0"/>
     </row>
@@ -17351,7 +17360,7 @@
         <v>55</v>
       </c>
       <c r="B588" s="2" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="C588" s="2" t="n">
         <v>1992</v>
@@ -17366,7 +17375,7 @@
         <v>4.25</v>
       </c>
       <c r="I588" s="2" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="J588" s="0"/>
     </row>
@@ -17375,7 +17384,7 @@
         <v>55</v>
       </c>
       <c r="B589" s="2" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="C589" s="2" t="n">
         <v>1996</v>
@@ -17390,7 +17399,7 @@
         <v>4.75</v>
       </c>
       <c r="I589" s="2" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="J589" s="0"/>
     </row>
@@ -17399,7 +17408,7 @@
         <v>55</v>
       </c>
       <c r="B590" s="2" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="C590" s="2" t="n">
         <v>1997</v>
@@ -17414,7 +17423,7 @@
         <v>5.15</v>
       </c>
       <c r="I590" s="2" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="J590" s="0"/>
     </row>
@@ -17423,7 +17432,7 @@
         <v>55</v>
       </c>
       <c r="B591" s="2" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="C591" s="2" t="n">
         <v>2005</v>
@@ -17438,7 +17447,7 @@
         <v>5.7</v>
       </c>
       <c r="I591" s="2" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="J591" s="0"/>
     </row>
@@ -17447,7 +17456,7 @@
         <v>55</v>
       </c>
       <c r="B592" s="2" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="C592" s="2" t="n">
         <v>2006</v>
@@ -17462,7 +17471,7 @@
         <v>6.5</v>
       </c>
       <c r="I592" s="2" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="J592" s="0"/>
     </row>
@@ -17471,7 +17480,7 @@
         <v>55</v>
       </c>
       <c r="B593" s="2" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="C593" s="2" t="n">
         <v>2009</v>
@@ -17486,7 +17495,7 @@
         <v>7.25</v>
       </c>
       <c r="I593" s="2" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="J593" s="0"/>
     </row>
@@ -17495,7 +17504,7 @@
         <v>55</v>
       </c>
       <c r="B594" s="2" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="C594" s="2" t="n">
         <v>2017</v>
@@ -17521,7 +17530,7 @@
         <v>56</v>
       </c>
       <c r="B595" s="2" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="C595" s="2" t="n">
         <v>2017</v>

</xml_diff>